<commit_message>
Enhance shopkeeper management: add brand field to UI and database queries; update fetch logic and UI components accordingly
</commit_message>
<xml_diff>
--- a/Backup/Shopkeepers.xlsx
+++ b/Backup/Shopkeepers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>IsDeleted</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Brand</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -472,6 +477,11 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Bonapapa</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -490,6 +500,11 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Candyland</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -508,6 +523,11 @@
       <c r="D4" t="n">
         <v>1</v>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Bonapapa</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -526,6 +546,11 @@
       <c r="D5" t="n">
         <v>1</v>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Candyland</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -544,6 +569,11 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Bonapapa</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -562,6 +592,11 @@
       <c r="D7" t="n">
         <v>0</v>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Candyland</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -579,6 +614,34 @@
       </c>
       <c r="D8" t="n">
         <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Bonapapa</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>9</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ahmed</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>53454634634</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Candyland</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>